<commit_message>
fix escaping in TeamCity output
</commit_message>
<xml_diff>
--- a/2.0/Documents/T10-Invoice/Tests/ValidationOverviewPEPPOL&BII_T10.xlsx
+++ b/2.0/Documents/T10-Invoice/Tests/ValidationOverviewPEPPOL&BII_T10.xlsx
@@ -72,6 +72,123 @@
     <t xml:space="preserve">Errors </t>
   </si>
   <si>
+    <t>EUGEN-T10-R041</t>
+  </si>
+  <si>
+    <t>T10-0011_EmptyElements_errors.xml</t>
+  </si>
+  <si>
+    <t>T10-0012-line_errors.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BII2-T10-R017
+ BII2-T10-R018
+ BII2-T10-R019
+ BII2-T10-R033
+ CL-T10-R003</t>
+  </si>
+  <si>
+    <t>T10-0013-negative_invoice_errors.xml</t>
+  </si>
+  <si>
+    <t>EUGEN-T10-R004</t>
+  </si>
+  <si>
+    <t>T10-0014-ErrorRounding_BIC_IBAN.xml</t>
+  </si>
+  <si>
+    <t>T10-0015-simpleINV_OK.xml</t>
+  </si>
+  <si>
+    <t>T10-0016-Valuta-EUR_Warn.xml</t>
+  </si>
+  <si>
+    <t>T10-0017-Standard_PEPPOL BIS_Warn.xml</t>
+  </si>
+  <si>
+    <t>T10-0018-OK2VATRatesSimple_OK.xml</t>
+  </si>
+  <si>
+    <t>T10-0019-RichContent_OK.xml</t>
+  </si>
+  <si>
+    <t>T10-0020-CrossBorder_OK.xml</t>
+  </si>
+  <si>
+    <t>T10-0021-EUVATNotAppicable_OK.xml</t>
+  </si>
+  <si>
+    <t>T10-0022-FullSpec_OK.xml</t>
+  </si>
+  <si>
+    <t>T10-0023-ErrorUOM.xml</t>
+  </si>
+  <si>
+    <t>T10-0024-ManyErrors.xml</t>
+  </si>
+  <si>
+    <t>T10-0025-CalcErrors.xml</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BIIRULES-UBL-T10.xsl </t>
+  </si>
+  <si>
+    <t>T10-0026-ReverseChargeERR.xml</t>
+  </si>
+  <si>
+    <t>T10-0027-MissVATCategory.xml</t>
+  </si>
+  <si>
+    <t>BII2-T10-R026</t>
+  </si>
+  <si>
+    <t>T10-0028-MissExemptReasonERR.xml</t>
+  </si>
+  <si>
+    <t>BII2-T10-R045</t>
+  </si>
+  <si>
+    <t>T10-0029-MissExemptReasonandVATOnLine.xml</t>
+  </si>
+  <si>
+    <t>[EUGEN-T10-R040]</t>
+  </si>
+  <si>
+    <t>PEPPOL</t>
+  </si>
+  <si>
+    <t>SCHEMATRON</t>
+  </si>
+  <si>
+    <t>DOC. TYPE</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>TEST-LINES</t>
+  </si>
+  <si>
+    <t>[BII2-T10-R026]</t>
+  </si>
+  <si>
+    <t>[BII2-T10-R030]
+[BII2-T10-R045]</t>
+  </si>
+  <si>
+    <t>[EUGEN-T10-R026]
+[EUGEN-T10-R046]</t>
+  </si>
+  <si>
+    <t>[CL-T10-R001] 
+[CL-T10-R002] 
+[CL-T10-R004] 
+[CL-T10-R003] 
+[CL-[T10-R007] 
+[CL-T10-R006]
+[OP-T10-R004]</t>
+  </si>
+  <si>
     <t>BII2-T10-R010
 BII2-T10-R011
 BII2-T10-R012
@@ -79,143 +196,37 @@
 BII2-T10-R039
 BII2-T10-R044
 BII2-T10-R051
-EUGEN-T10-R024 x 2
+EUGEN-T10-R024
 EUGEN-T10-R043</t>
   </si>
   <si>
-    <t>EUGEN-T10-R041</t>
-  </si>
-  <si>
-    <t>T10-0011_EmptyElements_errors.xml</t>
-  </si>
-  <si>
-    <t>T10-0012-line_errors.xml</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> BII2-T10-R017
- BII2-T10-R018
- BII2-T10-R019
- BII2-T10-R033
- CL-T10-R003</t>
-  </si>
-  <si>
-    <t>T10-0013-negative_invoice_errors.xml</t>
-  </si>
-  <si>
-    <t>EUGEN-T10-R004</t>
-  </si>
-  <si>
-    <t>T10-0014-ErrorRounding_BIC_IBAN.xml</t>
-  </si>
-  <si>
-    <t>T10-0015-simpleINV_OK.xml</t>
-  </si>
-  <si>
-    <t>T10-0016-Valuta-EUR_Warn.xml</t>
-  </si>
-  <si>
-    <t>T10-0017-Standard_PEPPOL BIS_Warn.xml</t>
-  </si>
-  <si>
-    <t>T10-0018-OK2VATRatesSimple_OK.xml</t>
-  </si>
-  <si>
-    <t>T10-0019-RichContent_OK.xml</t>
-  </si>
-  <si>
-    <t>T10-0020-CrossBorder_OK.xml</t>
-  </si>
-  <si>
-    <t>T10-0021-EUVATNotAppicable_OK.xml</t>
-  </si>
-  <si>
-    <t>T10-0022-FullSpec_OK.xml</t>
-  </si>
-  <si>
-    <t>T10-0023-ErrorUOM.xml</t>
-  </si>
-  <si>
-    <t>T10-0024-ManyErrors.xml</t>
-  </si>
-  <si>
-    <t>T10-0025-CalcErrors.xml</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BIIRULES-UBL-T10.xsl </t>
-  </si>
-  <si>
-    <t xml:space="preserve">BII2-T10-R051
+    <t>[BII2-T10-R042]
+[BII2-T10-R040]</t>
+  </si>
+  <si>
+    <t>[BII2-T10-R018] 
+[BII2-T10-R019]</t>
+  </si>
+  <si>
+    <t>BII2-T10-R030
+BII2-T10-R045
+BII2-T10-R018
+BII2-T10-R019</t>
+  </si>
+  <si>
+    <t>BII2-T10-R051
 BII2-T10-R052
-BII2-T10-R018 x 5
-BII2-T10-R019 x 5
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BII2-T10-R030
-BII2-T10-R045
-BII2-T10-R018 x 5
-BII2-T10-R019 x 5
-</t>
-  </si>
-  <si>
-    <t>T10-0026-ReverseChargeERR.xml</t>
-  </si>
-  <si>
-    <t>T10-0027-MissVATCategory.xml</t>
-  </si>
-  <si>
-    <t>BII2-T10-R026</t>
-  </si>
-  <si>
-    <t>T10-0028-MissExemptReasonERR.xml</t>
-  </si>
-  <si>
-    <t>BII2-T10-R045</t>
-  </si>
-  <si>
-    <t>T10-0029-MissExemptReasonandVATOnLine.xml</t>
-  </si>
-  <si>
-    <t>[EUGEN-T10-R040]</t>
-  </si>
-  <si>
-    <t>PEPPOL</t>
-  </si>
-  <si>
-    <t>SCHEMATRON</t>
-  </si>
-  <si>
-    <t>DOC. TYPE</t>
-  </si>
-  <si>
-    <t>T10</t>
-  </si>
-  <si>
-    <t>TEST-LINES</t>
-  </si>
-  <si>
-    <t>[BII2-T10-R026]</t>
-  </si>
-  <si>
-    <t>[BII2-T10-R030] [BII2-T10-R045]</t>
-  </si>
-  <si>
-    <t>[CL-T10-R001] [CL-T10-R002] [CL-T10-R004] [CL-T10-R003] [CL-[T10-R007] [CL-T10-R006] [OP-T10-R004]</t>
-  </si>
-  <si>
-    <t>[BII2-T10-R042] [BII2-T10-R040]</t>
-  </si>
-  <si>
-    <t>[BII2-T10-R018] [BII2-T10-R019]</t>
-  </si>
-  <si>
-    <t>[BII2-T10-R045] [BII2-T10-R046]</t>
-  </si>
-  <si>
-    <t>[BII2-T10-R047] [BII2-T10-R048] [BII2-T10-R045]</t>
-  </si>
-  <si>
-    <t>[EUGEN-T10-R026] [EUGEN-T10-R046]</t>
+BII2-T10-R018
+BII2-T10-R019</t>
+  </si>
+  <si>
+    <t>[BII2-T10-R047] 
+[BII2-T10-R048] 
+[BII2-T10-R045]</t>
+  </si>
+  <si>
+    <t>[BII2-T10-R045] 
+[BII2-T10-R046]</t>
   </si>
 </sst>
 </file>
@@ -578,7 +589,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +599,7 @@
     <col min="3" max="3" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="15.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="1"/>
     <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -597,13 +608,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
@@ -616,66 +627,66 @@
         <v>10</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f>A2 &amp; "; " &amp; B2 &amp; "; " &amp; C2 &amp; "; " &amp; F2</f>
+        <f>A2 &amp; "; " &amp; B2 &amp; "; " &amp; C2 &amp; "; " &amp; SUBSTITUTE(F2,CHAR(10), " ")</f>
         <v>PEPPOL; T10-0001-BII04 minimal invoice_errorVAT.xml; T10; [BII2-T10-R026]</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f t="shared" ref="I3:I29" si="0">A3 &amp; "; " &amp; B3 &amp; "; " &amp; C3 &amp; "; " &amp; F3</f>
+        <f t="shared" ref="I3:I29" si="0">A3 &amp; "; " &amp; B3 &amp; "; " &amp; C3 &amp; "; " &amp; SUBSTITUTE(F3,CHAR(10), " ")</f>
         <v>PEPPOL; T10-0002-minimal VAT invoice_ErrorVAT.xml; T10; [BII2-T10-R030] [BII2-T10-R045]</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
@@ -690,13 +701,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
@@ -711,46 +722,46 @@
     </row>
     <row r="6" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PEPPOL; T10-0005-MultipleSchematronErrors.xml; T10; [CL-T10-R001] [CL-T10-R002] [CL-T10-R004] [CL-T10-R003] [CL-[T10-R007] [CL-T10-R006] [OP-T10-R004]</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>PEPPOL; T10-0005-MultipleSchematronErrors.xml; T10; [CL-T10-R001]  [CL-T10-R002]  [CL-T10-R004]  [CL-T10-R003]  [CL-[T10-R007]  [CL-T10-R006] [OP-T10-R004]</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -759,13 +770,13 @@
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>9</v>
@@ -780,13 +791,13 @@
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>9</v>
@@ -801,13 +812,13 @@
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>9</v>
@@ -823,75 +834,63 @@
         <v>PEPPOL; T10-0010-B2C_error.xml; T10; OP-T10-R004</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="I11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PEPPOL; T10-0011_EmptyElements_errors.xml; T10; BII2-T10-R010
-BII2-T10-R011
-BII2-T10-R012
-BII2-T10-R013
-BII2-T10-R039
-BII2-T10-R044
-BII2-T10-R051
-EUGEN-T10-R024 x 2
-EUGEN-T10-R043</v>
+        <v>PEPPOL; T10-0011_EmptyElements_errors.xml; T10; BII2-T10-R010 BII2-T10-R011 BII2-T10-R012 BII2-T10-R013 BII2-T10-R039 BII2-T10-R044 BII2-T10-R051 EUGEN-T10-R024 EUGEN-T10-R043</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PEPPOL; T10-0012-line_errors.xml; T10;  BII2-T10-R017
- BII2-T10-R018
- BII2-T10-R019
- BII2-T10-R033
- CL-T10-R003</v>
+        <v>PEPPOL; T10-0012-line_errors.xml; T10;  BII2-T10-R017  BII2-T10-R018  BII2-T10-R019  BII2-T10-R033  CL-T10-R003</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>9</v>
@@ -906,22 +905,22 @@
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -930,13 +929,13 @@
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>9</v>
@@ -951,19 +950,19 @@
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -972,13 +971,13 @@
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>9</v>
@@ -993,13 +992,13 @@
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>9</v>
@@ -1014,13 +1013,13 @@
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>9</v>
@@ -1035,13 +1034,13 @@
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>9</v>
@@ -1056,13 +1055,13 @@
     </row>
     <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>9</v>
@@ -1077,13 +1076,13 @@
     </row>
     <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>9</v>
@@ -1098,96 +1097,88 @@
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>PEPPOL; T10-0023-ErrorUOM.xml; T10; [BII2-T10-R018]  [BII2-T10-R019]</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="2" t="s">
+      <c r="C24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I23" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>PEPPOL; T10-0023-ErrorUOM.xml; T10; [BII2-T10-R018] [BII2-T10-R019]</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="1" t="s">
+      <c r="G24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>PEPPOL; T10-0024-ManyErrors.xml; T10; BII2-T10-R030 BII2-T10-R045 BII2-T10-R018 BII2-T10-R019</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0024-ManyErrors.xml; T10; BII2-T10-R030
-BII2-T10-R045
-BII2-T10-R018 x 5
-BII2-T10-R019 x 5
-</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0025-CalcErrors.xml; T10; BII2-T10-R051
-BII2-T10-R052
-BII2-T10-R018 x 5
-BII2-T10-R019 x 5
-</v>
+        <v>PEPPOL; T10-0025-CalcErrors.xml; T10; BII2-T10-R051 BII2-T10-R052 BII2-T10-R018 BII2-T10-R019</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>58</v>
@@ -1197,24 +1188,24 @@
       </c>
       <c r="I26" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PEPPOL; T10-0026-ReverseChargeERR.xml; T10; [BII2-T10-R047] [BII2-T10-R048] [BII2-T10-R045]</v>
+        <v>PEPPOL; T10-0026-ReverseChargeERR.xml; T10; [BII2-T10-R047]  [BII2-T10-R048]  [BII2-T10-R045]</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>5</v>
@@ -1226,19 +1217,19 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>5</v>
@@ -1250,26 +1241,26 @@
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I29" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PEPPOL; T10-0029-MissExemptReasonandVATOnLine.xml; T10; [BII2-T10-R045] [BII2-T10-R046]</v>
+        <v>PEPPOL; T10-0029-MissExemptReasonandVATOnLine.xml; T10; [BII2-T10-R045]  [BII2-T10-R046]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
also output the schematron output
</commit_message>
<xml_diff>
--- a/2.0/Documents/T10-Invoice/Tests/ValidationOverviewPEPPOL&BII_T10.xlsx
+++ b/2.0/Documents/T10-Invoice/Tests/ValidationOverviewPEPPOL&BII_T10.xlsx
@@ -163,9 +163,6 @@
     <t>T10</t>
   </si>
   <si>
-    <t>TEST-LINES</t>
-  </si>
-  <si>
     <t>[BII2-T10-R026]</t>
   </si>
   <si>
@@ -224,6 +221,9 @@
   <si>
     <t>[BII2-T10-R045] 
 [BII2-T10-R046]</t>
+  </si>
+  <si>
+    <t>TEST-LINES for the test-config.txt file</t>
   </si>
 </sst>
 </file>
@@ -586,7 +586,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +599,7 @@
     <col min="6" max="6" width="18.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="60.42578125" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -624,7 +624,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -641,7 +641,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I2" s="1" t="str">
         <f>A2 &amp; "; " &amp; B2 &amp; "; " &amp; C2 &amp; "; " &amp; SUBSTITUTE(F2,CHAR(10), " ") &amp; " " &amp; SUBSTITUTE(G2,CHAR(10), " ")</f>
@@ -662,7 +662,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I3" s="1" t="str">
         <f t="shared" ref="I3:I29" si="0">A3 &amp; "; " &amp; B3 &amp; "; " &amp; C3 &amp; "; " &amp; SUBSTITUTE(F3,CHAR(10), " ") &amp; " " &amp; SUBSTITUTE(G3,CHAR(10), " ")</f>
@@ -719,7 +719,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -740,7 +740,7 @@
         <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>42</v>
@@ -824,7 +824,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>17</v>
@@ -890,7 +890,7 @@
         <v>8</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>22</v>
@@ -1064,7 +1064,7 @@
         <v>35</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1085,7 +1085,7 @@
         <v>35</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I24" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1106,7 +1106,7 @@
         <v>35</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I25" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1127,7 +1127,7 @@
         <v>35</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I26" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1190,7 +1190,7 @@
         <v>35</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I29" s="1" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Split BII and OPENPEPPOL tests
</commit_message>
<xml_diff>
--- a/2.0/Documents/T10-Invoice/Tests/ValidationOverviewPEPPOL&BII_T10.xlsx
+++ b/2.0/Documents/T10-Invoice/Tests/ValidationOverviewPEPPOL&BII_T10.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="62">
   <si>
     <t xml:space="preserve">File Name </t>
   </si>
@@ -151,9 +151,6 @@
     <t>[EUGEN-T10-R040]</t>
   </si>
   <si>
-    <t>PEPPOL</t>
-  </si>
-  <si>
     <t>SCHEMATRON</t>
   </si>
   <si>
@@ -172,6 +169,44 @@
   <si>
     <t>[EUGEN-T10-R026]
 [EUGEN-T10-R046]</t>
+  </si>
+  <si>
+    <t>[BII2-T10-R042]
+[BII2-T10-R040]</t>
+  </si>
+  <si>
+    <t>[BII2-T10-R018] 
+[BII2-T10-R019]</t>
+  </si>
+  <si>
+    <t>BII2-T10-R030
+BII2-T10-R045
+BII2-T10-R018
+BII2-T10-R019</t>
+  </si>
+  <si>
+    <t>BII2-T10-R051
+BII2-T10-R052
+BII2-T10-R018
+BII2-T10-R019</t>
+  </si>
+  <si>
+    <t>[BII2-T10-R047] 
+[BII2-T10-R048] 
+[BII2-T10-R045]</t>
+  </si>
+  <si>
+    <t>[BII2-T10-R045] 
+[BII2-T10-R046]</t>
+  </si>
+  <si>
+    <t>TEST-LINES for the test-config.txt file</t>
+  </si>
+  <si>
+    <t>OPENPEPPOL</t>
+  </si>
+  <si>
+    <t>BIIRULES</t>
   </si>
   <si>
     <t>[CL-T10-R001] 
@@ -179,8 +214,10 @@
 [CL-T10-R004] 
 [CL-T10-R003] 
 [CL-[T10-R007] 
-[CL-T10-R006]
-[OP-T10-R004]</t>
+[CL-T10-R006]</t>
+  </si>
+  <si>
+    <t>[OP-T10-R004]</t>
   </si>
   <si>
     <t>BII2-T10-R010
@@ -189,41 +226,11 @@
 BII2-T10-R013
 BII2-T10-R039
 BII2-T10-R044
-BII2-T10-R051
-EUGEN-T10-R024
+BII2-T10-R051</t>
+  </si>
+  <si>
+    <t>EUGEN-T10-R024
 EUGEN-T10-R043</t>
-  </si>
-  <si>
-    <t>[BII2-T10-R042]
-[BII2-T10-R040]</t>
-  </si>
-  <si>
-    <t>[BII2-T10-R018] 
-[BII2-T10-R019]</t>
-  </si>
-  <si>
-    <t>BII2-T10-R030
-BII2-T10-R045
-BII2-T10-R018
-BII2-T10-R019</t>
-  </si>
-  <si>
-    <t>BII2-T10-R051
-BII2-T10-R052
-BII2-T10-R018
-BII2-T10-R019</t>
-  </si>
-  <si>
-    <t>[BII2-T10-R047] 
-[BII2-T10-R048] 
-[BII2-T10-R045]</t>
-  </si>
-  <si>
-    <t>[BII2-T10-R045] 
-[BII2-T10-R046]</t>
-  </si>
-  <si>
-    <t>TEST-LINES for the test-config.txt file</t>
   </si>
 </sst>
 </file>
@@ -582,11 +589,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,13 +612,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
@@ -624,577 +631,678 @@
         <v>9</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" s="1" t="str">
         <f>A2 &amp; "; " &amp; B2 &amp; "; " &amp; C2 &amp; "; " &amp; SUBSTITUTE(F2,CHAR(10), " ") &amp; " " &amp; SUBSTITUTE(G2,CHAR(10), " ")</f>
-        <v xml:space="preserve">PEPPOL; T10-0001-BII04 minimal invoice_errorVAT.xml; T10; [BII2-T10-R026] </v>
+        <v xml:space="preserve">BIIRULES; T10-0001-BII04 minimal invoice_errorVAT.xml; T10; [BII2-T10-R026] </v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I3" s="1" t="str">
-        <f t="shared" ref="I3:I29" si="0">A3 &amp; "; " &amp; B3 &amp; "; " &amp; C3 &amp; "; " &amp; SUBSTITUTE(F3,CHAR(10), " ") &amp; " " &amp; SUBSTITUTE(G3,CHAR(10), " ")</f>
-        <v xml:space="preserve">PEPPOL; T10-0002-minimal VAT invoice_ErrorVAT.xml; T10; [BII2-T10-R030] [BII2-T10-R045] </v>
+        <f t="shared" ref="I3:I34" si="0">A3 &amp; "; " &amp; B3 &amp; "; " &amp; C3 &amp; "; " &amp; SUBSTITUTE(F3,CHAR(10), " ") &amp; " " &amp; SUBSTITUTE(G3,CHAR(10), " ")</f>
+        <v xml:space="preserve">BIIRULES; T10-0002-minimal VAT invoice_ErrorVAT.xml; T10; [BII2-T10-R030] [BII2-T10-R045] </v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0003-full core data_OK.xml; T10;  </v>
+        <v xml:space="preserve">BIIRULES; T10-0003-full core data_OK.xml; T10;  </v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0004-example common data_OK.xml; T10;  </v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I5" si="1">A5 &amp; "; " &amp; B5 &amp; "; " &amp; C5 &amp; "; " &amp; SUBSTITUTE(F5,CHAR(10), " ") &amp; " " &amp; SUBSTITUTE(G5,CHAR(10), " ")</f>
+        <v xml:space="preserve">OPENPEPPOL; T10-0003-full core data_OK.xml; T10;  </v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">OPENPEPPOL; T10-0004-example common data_OK.xml; T10;  </v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0005-MultipleSchematronErrors.xml; T10; [CL-T10-R001]  [CL-T10-R002]  [CL-T10-R004]  [CL-T10-R003]  [CL-[T10-R007]  [CL-T10-R006] [OP-T10-R004] </v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="I7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PEPPOL; T10-0006-MultipleCurrencies_error.xml; T10; [EUGEN-T10-R026] [EUGEN-T10-R046] [EUGEN-T10-R040]</v>
+        <v xml:space="preserve">BIIRULES; T10-0005-MultipleSchematronErrors.xml; T10; [CL-T10-R001]  [CL-T10-R002]  [CL-T10-R004]  [CL-T10-R003]  [CL-[T10-R007]  [CL-T10-R006] </v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F8" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="I8" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0007-RoundingAmount_OK.xml; T10;  </v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I8" si="2">A8 &amp; "; " &amp; B8 &amp; "; " &amp; C8 &amp; "; " &amp; SUBSTITUTE(F8,CHAR(10), " ") &amp; " " &amp; SUBSTITUTE(G8,CHAR(10), " ")</f>
+        <v xml:space="preserve">OPENPEPPOL; T10-0005-MultipleSchematronErrors.xml; T10; [OP-T10-R004] </v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="I9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0009-FullSpecINV.xml; T10;  </v>
+        <v>OPENPEPPOL; T10-0006-MultipleCurrencies_error.xml; T10; [EUGEN-T10-R026] [EUGEN-T10-R046] [EUGEN-T10-R040]</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">OPENPEPPOL; T10-0007-RoundingAmount_OK.xml; T10;  </v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">OPENPEPPOL; T10-0009-FullSpecINV.xml; T10;  </v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>PEPPOL; T10-0010-B2C_error.xml; T10; OP-T10-R004 EUGEN-T10-R040</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>OPENPEPPOL; T10-0010-B2C_error.xml; T10; OP-T10-R004 EUGEN-T10-R040</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>PEPPOL; T10-0011_EmptyElements_errors.xml; T10; BII2-T10-R010 BII2-T10-R011 BII2-T10-R012 BII2-T10-R013 BII2-T10-R039 BII2-T10-R044 BII2-T10-R051 EUGEN-T10-R024 EUGEN-T10-R043 EUGEN-T10-R041</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>PEPPOL; T10-0012-line_errors.xml; T10;  BII2-T10-R017  BII2-T10-R018  BII2-T10-R019  BII2-T10-R033  CL-T10-R003 EUGEN-T10-R041</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F13" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="I13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0013-negative_invoice_errors.xml; T10;  </v>
+        <v xml:space="preserve">BIIRULES; T10-0011_EmptyElements_errors.xml; T10; BII2-T10-R010 BII2-T10-R011 BII2-T10-R012 BII2-T10-R013 BII2-T10-R039 BII2-T10-R044 BII2-T10-R051 </v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>52</v>
-      </c>
+      <c r="F14" s="3"/>
       <c r="G14" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I14" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>PEPPOL; T10-0014-ErrorRounding_BIC_IBAN.xml; T10; [BII2-T10-R042] [BII2-T10-R040] EUGEN-T10-R004</v>
+        <f t="shared" ref="I14" si="3">A14 &amp; "; " &amp; B14 &amp; "; " &amp; C14 &amp; "; " &amp; SUBSTITUTE(F14,CHAR(10), " ") &amp; " " &amp; SUBSTITUTE(G14,CHAR(10), " ")</f>
+        <v>OPENPEPPOL; T10-0011_EmptyElements_errors.xml; T10;  EUGEN-T10-R041</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I15" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0015-simpleINV_OK.xml; T10;  </v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <f t="shared" ref="I15" si="4">A15 &amp; "; " &amp; B15 &amp; "; " &amp; C15 &amp; "; " &amp; SUBSTITUTE(F15,CHAR(10), " ") &amp; " " &amp; SUBSTITUTE(G15,CHAR(10), " ")</f>
+        <v>OPENPEPPOL; T10-0011_EmptyElements_errors.xml; T10; EUGEN-T10-R024 EUGEN-T10-R043 EUGEN-T10-R041</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PEPPOL; T10-0016-Valuta-EUR_Warn.xml; T10;  EUGEN-T10-R041</v>
+        <v>BIIRULES; T10-0012-line_errors.xml; T10;  BII2-T10-R017  BII2-T10-R018  BII2-T10-R019  BII2-T10-R033  CL-T10-R003 EUGEN-T10-R041</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="I17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>PEPPOL; T10-0017-Standard_PEPPOL BIS_Warn.xml; T10;  EUGEN-T10-R040</v>
+        <v xml:space="preserve">OPENPEPPOL; T10-0013-negative_invoice_errors.xml; T10;  </v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F18" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="I18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0018-OK2VATRatesSimple_OK.xml; T10;  </v>
+        <v xml:space="preserve">BIIRULES; T10-0014-ErrorRounding_BIC_IBAN.xml; T10; [BII2-T10-R042] [BII2-T10-R040] </v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="I19" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0019-RichContent_OK.xml; T10;  </v>
+        <f t="shared" ref="I19" si="5">A19 &amp; "; " &amp; B19 &amp; "; " &amp; C19 &amp; "; " &amp; SUBSTITUTE(F19,CHAR(10), " ") &amp; " " &amp; SUBSTITUTE(G19,CHAR(10), " ")</f>
+        <v>OPENPEPPOL; T10-0014-ErrorRounding_BIC_IBAN.xml; T10;  EUGEN-T10-R004</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0020-CrossBorder_OK.xml; T10;  </v>
+        <v xml:space="preserve">OPENPEPPOL; T10-0015-simpleINV_OK.xml; T10;  </v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G21" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="I21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0021-EUVATNotAppicable_OK.xml; T10;  </v>
+        <v>OPENPEPPOL; T10-0016-Valuta-EUR_Warn.xml; T10;  EUGEN-T10-R041</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G22" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="I22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0022-FullSpec_OK.xml; T10;  </v>
+        <v>OPENPEPPOL; T10-0017-Standard_PEPPOL BIS_Warn.xml; T10;  EUGEN-T10-R040</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">OPENPEPPOL; T10-0018-OK2VATRatesSimple_OK.xml; T10;  </v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">OPENPEPPOL; T10-0019-RichContent_OK.xml; T10;  </v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">OPENPEPPOL; T10-0020-CrossBorder_OK.xml; T10;  </v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">OPENPEPPOL; T10-0021-EUVATNotAppicable_OK.xml; T10;  </v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">OPENPEPPOL; T10-0022-FullSpec_OK.xml; T10;  </v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I23" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0023-ErrorUOM.xml; T10; [BII2-T10-R018]  [BII2-T10-R019] </v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0024-ManyErrors.xml; T10; BII2-T10-R030 BII2-T10-R045 BII2-T10-R018 BII2-T10-R019 </v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I25" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0025-CalcErrors.xml; T10; BII2-T10-R051 BII2-T10-R052 BII2-T10-R018 BII2-T10-R019 </v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I26" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0026-ReverseChargeERR.xml; T10; [BII2-T10-R047]  [BII2-T10-R048]  [BII2-T10-R045] </v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I27" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0027-MissVATCategory.xml; T10; BII2-T10-R026 </v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I28" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0028-MissExemptReasonERR.xml; T10; BII2-T10-R045 </v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">BIIRULES; T10-0023-ErrorUOM.xml; T10; [BII2-T10-R018]  [BII2-T10-R019] </v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>35</v>
       </c>
       <c r="F29" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">BIIRULES; T10-0024-ManyErrors.xml; T10; BII2-T10-R030 BII2-T10-R045 BII2-T10-R018 BII2-T10-R019 </v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I29" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">PEPPOL; T10-0029-MissExemptReasonandVATOnLine.xml; T10; [BII2-T10-R045]  [BII2-T10-R046] </v>
+      <c r="B30" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">BIIRULES; T10-0025-CalcErrors.xml; T10; BII2-T10-R051 BII2-T10-R052 BII2-T10-R018 BII2-T10-R019 </v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">BIIRULES; T10-0026-ReverseChargeERR.xml; T10; [BII2-T10-R047]  [BII2-T10-R048]  [BII2-T10-R045] </v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">BIIRULES; T10-0027-MissVATCategory.xml; T10; BII2-T10-R026 </v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">BIIRULES; T10-0028-MissExemptReasonERR.xml; T10; BII2-T10-R045 </v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">BIIRULES; T10-0029-MissExemptReasonandVATOnLine.xml; T10; [BII2-T10-R045]  [BII2-T10-R046] </v>
       </c>
     </row>
   </sheetData>

</xml_diff>